<commit_message>
feat(review): enhance ReviewDTO and ReviewServiceImpl to include product variant details and order code; update response structure for improved review data representation
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/category_import_template.xlsx
+++ b/src/main/resources/templates/excel/category_import_template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sturdyspace\nam 4\hk1\tlcn\ecommerce-fashion-tlcn\ecommerce-fashion-be\src\main\resources\templates\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sturdyspace\nam4\hk1\tlcn\ecommerce-fashion-tlcn\ecommerce-fashion-be\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10DA3E1-0A14-450F-8867-3050874A731C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8445518-6CFD-4412-82EF-4F0C9DB1AA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dữ liệu mẫu" sheetId="1" r:id="rId1"/>
+    <sheet name="Dữ liệu danh mục" sheetId="1" r:id="rId1"/>
     <sheet name="Hướng dẫn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -435,7 +435,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -555,7 +555,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
feat(import): integrate Pinecone indexing in ImportServiceImpl for product imports; enhance RecommendationServiceImpl to ensure limit compliance in recommended products
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/category_import_template.xlsx
+++ b/src/main/resources/templates/excel/category_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sturdyspace\nam4\hk1\tlcn\ecommerce-fashion-tlcn\ecommerce-fashion-be\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8445518-6CFD-4412-82EF-4F0C9DB1AA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA02DC-7675-4237-ACED-7C4025877036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dữ liệu danh mục" sheetId="1" r:id="rId1"/>
@@ -21,72 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Category Name (*)</t>
   </si>
   <si>
     <t>Category Image URL (*)</t>
-  </si>
-  <si>
-    <t>Áo Sơ Mi &amp; Áo Kiểu</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/ao-so-mi.png</t>
-  </si>
-  <si>
-    <t>Quần Jeans</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/quan-jean.png</t>
-  </si>
-  <si>
-    <t>Váy Đầm</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/vay-dam.png</t>
-  </si>
-  <si>
-    <t>Áo Khoác &amp; Áo Len</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/ao-khoac.png</t>
-  </si>
-  <si>
-    <t>Đồ Mặc Nhà</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/do-mac-nha.png</t>
-  </si>
-  <si>
-    <t>Phụ Kiện Thời Trang</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/phu-kien.png</t>
-  </si>
-  <si>
-    <t>Giày Dép Nữ</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/giay-dep.png</t>
-  </si>
-  <si>
-    <t>Túi Xách</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/tui-xach.png</t>
-  </si>
-  <si>
-    <t>Đồ Thể Thao Nữ</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/do-the-thao.png</t>
-  </si>
-  <si>
-    <t>Trang Sức</t>
-  </si>
-  <si>
-    <t>https://your.cloud/images/categories/trang-suc.png</t>
   </si>
   <si>
     <t>Mục</t>
@@ -123,13 +63,19 @@
   <si>
     <t>Tên danh mục sau khi import phải là duy nhất. Nếu tên danh mục đã tồn tại, dòng đó sẽ gây ra lỗi khi import (vì hiện tại chỉ hỗ trợ chế độ "ADD_ONLY").
 Đảm bảo URL hình ảnh là hợp lệ và có thể truy cập công khai.</t>
+  </si>
+  <si>
+    <t>Quần dài</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/db9vcatme/image/upload/v1749816289/quan-dai-removebg-preview_qk7y0r.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,6 +115,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -189,10 +142,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -215,8 +169,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,7 +393,9 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -451,98 +411,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -555,7 +470,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -565,42 +480,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>